<commit_message>
Added folder for Parsed Water Sensor Data
</commit_message>
<xml_diff>
--- a/Data_Flow_Team/SQL_Database/Data_Import/Progresses.xlsx
+++ b/Data_Flow_Team/SQL_Database/Data_Import/Progresses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amponcet/Documents/GitHub/CROWN/Data_Flow_Team/SQL_Database/Data_Import/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E35DD1-793E-6247-9785-AB71B8048C98}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ACB4C76-9ED3-5A42-9E13-FB1FD411B759}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2620" yWindow="460" windowWidth="23640" windowHeight="16260" xr2:uid="{872CB2A6-88F1-1B47-8023-944840A535F8}"/>
+    <workbookView xWindow="2620" yWindow="460" windowWidth="23640" windowHeight="16220" xr2:uid="{872CB2A6-88F1-1B47-8023-944840A535F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -201,7 +201,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -226,12 +226,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -245,7 +239,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -266,9 +260,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -587,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85B814E9-C816-1443-9A7B-0446A390B7A6}">
   <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41:B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -628,7 +619,7 @@
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="8"/>
+      <c r="B5" s="6"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -640,13 +631,13 @@
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="5"/>
+      <c r="B7" s="6"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="5"/>
+      <c r="B8" s="6"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
@@ -976,6 +967,22 @@
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
     </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="5"/>
+      <c r="L37" s="5"/>
+    </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>48</v>
@@ -985,16 +992,16 @@
       <c r="A41" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="B41" s="5"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="B42" s="5"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="A43" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>